<commit_message>
modificacion Lista de Productos/servicios
</commit_message>
<xml_diff>
--- a/Listado de Productos y Servicios.xlsx
+++ b/Listado de Productos y Servicios.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Producto/servicio</t>
   </si>
@@ -31,50 +31,78 @@
     <t>Costo</t>
   </si>
   <si>
-    <t>Radiodifusión</t>
+    <t>microfonos</t>
   </si>
   <si>
-    <t>por medio de streaming o emisión por internet en directo, así como la locución y entretenimiento del espectador</t>
+    <t>microfono SM-58 de Shure</t>
   </si>
   <si>
     <t>no aplica</t>
   </si>
   <si>
-    <t>Tiempo al aire</t>
+    <t>MXN1,967.00</t>
   </si>
   <si>
-    <t>$13.16/s</t>
+    <t>CPU</t>
   </si>
   <si>
-    <t>Programacion Musical</t>
+    <t>Equipo de computo con las siguientes capacidades minimas:
+procesador pentium 4
+2GB de memoria Ram
+Disco duro de 500GB</t>
   </si>
   <si>
-    <t>nuestra programación musical está especializada para el goce y disfrute del radioescucha</t>
+    <t>MNX8,999.00</t>
   </si>
   <si>
-    <t>Cancion</t>
+    <t>Servicio de internet</t>
   </si>
   <si>
-    <t>$10.00 p/cancion</t>
+    <t>Servicio con velocidad de  2.5mb  de subida</t>
   </si>
   <si>
-    <t>Locución</t>
+    <t>Mega bits</t>
   </si>
   <si>
-    <t>gracias a nuestros locutores altamente capacitados, es posible brindar servicios de difusión en la programación.</t>
+    <t>MNX389 /mes</t>
   </si>
   <si>
-    <t>Marketing</t>
+    <t>Audifonos</t>
   </si>
   <si>
-    <t>es posible contratar el servicio de marketing, que permite a su empresa darse a conocer mediante nuestra radiodifusora.</t>
+    <t xml:space="preserve"> monitores de frecuencia plana
+Behringer Truth B1030A</t>
+  </si>
+  <si>
+    <t>MNX6,249.00</t>
+  </si>
+  <si>
+    <t>tarjeta de audio</t>
+  </si>
+  <si>
+    <t>Mia Midi de Echo Audio
+entrada digital S/PDFI, midi, y multi-análogas.
+</t>
+  </si>
+  <si>
+    <t>MNX2,950.00</t>
+  </si>
+  <si>
+    <t>consola</t>
+  </si>
+  <si>
+    <t>Un mezclador de 4 ó 6 canales con ecualización incorporada, al menos en los canales de micrófonos
+</t>
+  </si>
+  <si>
+    <t>MNX3000.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -95,12 +123,16 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF222222"/>
       <name val="Arial"/>
     </font>
+    <font/>
+    <font>
+      <sz val="10.0"/>
+      <color rgb="FFFFFFFF"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -111,6 +143,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF1C4587"/>
         <bgColor rgb="FF1C4587"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -125,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -147,14 +185,23 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -230,17 +277,17 @@
       <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="7">
+        <v>42502.0</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>10</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -265,22 +312,22 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>12</v>
+      <c r="C3" s="6">
+        <v>1.0</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>8</v>
+      <c r="E3" s="7">
+        <v>42503.0</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -304,23 +351,23 @@
       <c r="Z3" s="3"/>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>8</v>
+      <c r="E4" s="7">
+        <v>42504.0</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -344,23 +391,23 @@
       <c r="Z4" s="3"/>
     </row>
     <row r="5">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>8</v>
+      <c r="C5" s="6">
+        <v>2.0</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>8</v>
+      <c r="E5" s="7">
+        <v>42505.0</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -383,13 +430,25 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
     </row>
-    <row r="6">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+    <row r="6" ht="43.5" customHeight="1">
+      <c r="A6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="7">
+        <v>42506.0</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -412,12 +471,24 @@
       <c r="Z6" s="3"/>
     </row>
     <row r="7">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="A7" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="7">
+        <v>42507.0</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>

</xml_diff>